<commit_message>
VCE Scenario updates to offshore wind and coal retirements by 2024
</commit_message>
<xml_diff>
--- a/InputData/elec/PMCCS/Pol Mandated Cap Const Sched.xlsx
+++ b/InputData/elec/PMCCS/Pol Mandated Cap Const Sched.xlsx
@@ -1,26 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Dropbox (Energy Innovation)\EPS Versions\eps-1.5.0-us-wipI - units progress\InputData\elec\PMCCS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Dropbox (Energy Innovation)\Documents\EPS_Models by Region\RMI\Virginia\Virginia_Model\InputData\elec\PMCCS\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45736304-2D9C-4081-AF78-56563B788BE6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="135" windowWidth="24915" windowHeight="11565"/>
+    <workbookView xWindow="8865" yWindow="465" windowWidth="17340" windowHeight="12825" activeTab="2" xr2:uid="{EDFD5CA4-AA4D-4A6A-B6B7-6C080971D85F}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
-    <sheet name="PMCCS" sheetId="2" r:id="rId2"/>
+    <sheet name="Required offshore wind" sheetId="3" r:id="rId2"/>
+    <sheet name="PMCCS" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="40">
   <si>
     <t>PMCCS Policy Mandated Capacity Construction Schedule</t>
   </si>
@@ -28,9 +40,6 @@
     <t>Source:</t>
   </si>
   <si>
-    <t>None (this variable is intended to be user-specified)</t>
-  </si>
-  <si>
     <t>Note:</t>
   </si>
   <si>
@@ -95,13 +104,65 @@
   </si>
   <si>
     <t>municipal solid waste</t>
+  </si>
+  <si>
+    <t>MW</t>
+  </si>
+  <si>
+    <t>offshore wind are within the public interest</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> (vi) establishes requirements regarding the development by Dominion Energy Virginia of qualified offshore wind projects having an aggregate rated capacity of not less than 5,200 megawatts by January 1, 2034, and provides that in constructing any such facility,</t>
+  </si>
+  <si>
+    <t>2024-2026</t>
+  </si>
+  <si>
+    <t>Virginia Clean Economy Act</t>
+  </si>
+  <si>
+    <t>Virginia's Legislative Information System</t>
+  </si>
+  <si>
+    <t>https://lis.virginia.gov/cgi-bin/legp604.exe?201+ful+CHAP1193</t>
+  </si>
+  <si>
+    <t>Pursuant to subsection B, construction by a Phase II Utility of one or more new utility-owned and utility-operated generating facilities utilizing energy derived from offshore wind and located off the Commonwealth's Atlantic shoreline, with an aggregate rated capacity of not less than 2,500 megawatts and not more than 3,000 megawatts, </t>
+  </si>
+  <si>
+    <t>Dominion offshore wind development</t>
+  </si>
+  <si>
+    <t>Greentech Media</t>
+  </si>
+  <si>
+    <t>https://www.greentechmedia.com/articles/read/dominion-plans-to-use-a-pilot-project-to-launch-an-offshore-wind-empire</t>
+  </si>
+  <si>
+    <t>Required Offshore Wind</t>
+  </si>
+  <si>
+    <t>Per year</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Dominion is currently building offshore wind and is approved to pass on costs to ratepayers. Project is projected to phase in 3 stages from 2024 to 2026</t>
+  </si>
+  <si>
+    <t>Required offshore wind (MW) Construction</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="169" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -117,13 +178,52 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF333333"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -135,14 +235,44 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -234,6 +364,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -269,6 +416,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -444,49 +608,96 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B5" s="7">
+        <v>43922</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B8" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B10" s="7">
+        <v>43952</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B11" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B12" s="7"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -496,14 +707,541 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8F4724C-7E44-4AA7-94EC-790A012325F5}">
+  <dimension ref="A1:K47"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.5703125" customWidth="1"/>
+    <col min="2" max="2" width="25.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+    </row>
+    <row r="2" spans="1:11" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="9"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7">
+        <v>2600</v>
+      </c>
+      <c r="C7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>2026</v>
+      </c>
+      <c r="B8">
+        <v>2600</v>
+      </c>
+      <c r="C8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="10"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>2035</v>
+      </c>
+      <c r="B9">
+        <v>5200</v>
+      </c>
+      <c r="C9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="2"/>
+    </row>
+    <row r="12" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="B12" s="12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>2017</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>2018</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>2019</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>2020</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>2021</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>2022</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>2023</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>2024</v>
+      </c>
+      <c r="B21" s="11">
+        <f>C21</f>
+        <v>866.66666666666663</v>
+      </c>
+      <c r="C21" s="14">
+        <v>866.66666666666663</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>2025</v>
+      </c>
+      <c r="B22" s="11">
+        <f>C22-C21</f>
+        <v>866.66666666666663</v>
+      </c>
+      <c r="C22" s="14">
+        <v>1733.3333333333333</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>2026</v>
+      </c>
+      <c r="B23" s="11">
+        <f t="shared" ref="B23:B32" si="0">C23-C22</f>
+        <v>866.66666666666674</v>
+      </c>
+      <c r="C23" s="14">
+        <v>2600</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>2027</v>
+      </c>
+      <c r="B24" s="11">
+        <f t="shared" si="0"/>
+        <v>288.88888888887595</v>
+      </c>
+      <c r="C24" s="14">
+        <f>_xlfn.FORECAST.LINEAR(A24,$B$8:$B$9,$A$8:$A$9)</f>
+        <v>2888.888888888876</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>2028</v>
+      </c>
+      <c r="B25" s="11">
+        <f t="shared" si="0"/>
+        <v>288.88888888887595</v>
+      </c>
+      <c r="C25" s="14">
+        <f t="shared" ref="C25:C32" si="1">_xlfn.FORECAST.LINEAR(A25,$B$8:$B$9,$A$8:$A$9)</f>
+        <v>3177.7777777777519</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>2029</v>
+      </c>
+      <c r="B26" s="11">
+        <f t="shared" si="0"/>
+        <v>288.88888888887595</v>
+      </c>
+      <c r="C26" s="14">
+        <f t="shared" si="1"/>
+        <v>3466.6666666666279</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>2030</v>
+      </c>
+      <c r="B27" s="11">
+        <f t="shared" si="0"/>
+        <v>288.88888888887595</v>
+      </c>
+      <c r="C27" s="14">
+        <f t="shared" si="1"/>
+        <v>3755.5555555555038</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>2031</v>
+      </c>
+      <c r="B28" s="11">
+        <f t="shared" si="0"/>
+        <v>288.88888888887595</v>
+      </c>
+      <c r="C28" s="14">
+        <f t="shared" si="1"/>
+        <v>4044.4444444443798</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>2032</v>
+      </c>
+      <c r="B29" s="11">
+        <f t="shared" si="0"/>
+        <v>288.88888888887595</v>
+      </c>
+      <c r="C29" s="14">
+        <f t="shared" si="1"/>
+        <v>4333.3333333332557</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>2033</v>
+      </c>
+      <c r="B30" s="11">
+        <f t="shared" si="0"/>
+        <v>288.88888888887595</v>
+      </c>
+      <c r="C30" s="14">
+        <f t="shared" si="1"/>
+        <v>4622.2222222221317</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>2034</v>
+      </c>
+      <c r="B31" s="11">
+        <f t="shared" si="0"/>
+        <v>288.88888888887595</v>
+      </c>
+      <c r="C31" s="14">
+        <f t="shared" si="1"/>
+        <v>4911.1111111110076</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>2035</v>
+      </c>
+      <c r="B32" s="11">
+        <f t="shared" si="0"/>
+        <v>288.88888888899237</v>
+      </c>
+      <c r="C32" s="14">
+        <f t="shared" si="1"/>
+        <v>5200</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>2036</v>
+      </c>
+      <c r="B33">
+        <v>0</v>
+      </c>
+      <c r="C33" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>2037</v>
+      </c>
+      <c r="B34">
+        <v>0</v>
+      </c>
+      <c r="C34" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>2038</v>
+      </c>
+      <c r="B35">
+        <v>0</v>
+      </c>
+      <c r="C35" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>2039</v>
+      </c>
+      <c r="B36">
+        <v>0</v>
+      </c>
+      <c r="C36" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>2040</v>
+      </c>
+      <c r="B37">
+        <v>0</v>
+      </c>
+      <c r="C37" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>2041</v>
+      </c>
+      <c r="B38">
+        <v>0</v>
+      </c>
+      <c r="C38" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>2042</v>
+      </c>
+      <c r="B39">
+        <v>0</v>
+      </c>
+      <c r="C39" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>2043</v>
+      </c>
+      <c r="B40">
+        <v>0</v>
+      </c>
+      <c r="C40" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>2044</v>
+      </c>
+      <c r="B41">
+        <v>0</v>
+      </c>
+      <c r="C41" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>2045</v>
+      </c>
+      <c r="B42">
+        <v>0</v>
+      </c>
+      <c r="C42" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>2046</v>
+      </c>
+      <c r="B43">
+        <v>0</v>
+      </c>
+      <c r="C43" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>2047</v>
+      </c>
+      <c r="B44">
+        <v>0</v>
+      </c>
+      <c r="C44" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>2048</v>
+      </c>
+      <c r="B45">
+        <v>0</v>
+      </c>
+      <c r="C45" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>2049</v>
+      </c>
+      <c r="B46">
+        <v>0</v>
+      </c>
+      <c r="C46" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>2050</v>
+      </c>
+      <c r="B47">
+        <v>0</v>
+      </c>
+      <c r="C47" s="13">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:AI17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -513,7 +1251,7 @@
   <sheetData>
     <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B1">
         <v>2017</v>
@@ -620,7 +1358,7 @@
     </row>
     <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -727,7 +1465,7 @@
     </row>
     <row r="3" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -834,7 +1572,7 @@
     </row>
     <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -941,7 +1679,7 @@
     </row>
     <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -1048,7 +1786,7 @@
     </row>
     <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -1155,7 +1893,7 @@
     </row>
     <row r="7" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -1262,7 +2000,7 @@
     </row>
     <row r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -1369,7 +2107,7 @@
     </row>
     <row r="9" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -1476,7 +2214,7 @@
     </row>
     <row r="10" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -1583,7 +2321,7 @@
     </row>
     <row r="11" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -1690,7 +2428,7 @@
     </row>
     <row r="12" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -1797,7 +2535,7 @@
     </row>
     <row r="13" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -1904,9 +2642,10 @@
     </row>
     <row r="14" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B14">
+        <f t="array" ref="B14:AI14">TRANSPOSE('Required offshore wind'!$B$14:$B$47)</f>
         <v>0</v>
       </c>
       <c r="C14">
@@ -1928,40 +2667,40 @@
         <v>0</v>
       </c>
       <c r="I14">
-        <v>0</v>
+        <v>866.66666666666663</v>
       </c>
       <c r="J14">
-        <v>0</v>
+        <v>866.66666666666663</v>
       </c>
       <c r="K14">
-        <v>0</v>
+        <v>866.66666666666674</v>
       </c>
       <c r="L14">
-        <v>0</v>
+        <v>288.88888888887595</v>
       </c>
       <c r="M14">
-        <v>0</v>
+        <v>288.88888888887595</v>
       </c>
       <c r="N14">
-        <v>0</v>
+        <v>288.88888888887595</v>
       </c>
       <c r="O14">
-        <v>0</v>
+        <v>288.88888888887595</v>
       </c>
       <c r="P14">
-        <v>0</v>
+        <v>288.88888888887595</v>
       </c>
       <c r="Q14">
-        <v>0</v>
+        <v>288.88888888887595</v>
       </c>
       <c r="R14">
-        <v>0</v>
+        <v>288.88888888887595</v>
       </c>
       <c r="S14">
-        <v>0</v>
+        <v>288.88888888887595</v>
       </c>
       <c r="T14">
-        <v>0</v>
+        <v>288.88888888899237</v>
       </c>
       <c r="U14">
         <v>0</v>
@@ -2011,7 +2750,7 @@
     </row>
     <row r="15" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -2118,7 +2857,7 @@
     </row>
     <row r="16" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -2225,7 +2964,7 @@
     </row>
     <row r="17" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B17">
         <v>0</v>

</xml_diff>

<commit_message>
Adjust offshore wind deployment for VCEA scenario
</commit_message>
<xml_diff>
--- a/InputData/elec/PMCCS/Pol Mandated Cap Const Sched.xlsx
+++ b/InputData/elec/PMCCS/Pol Mandated Cap Const Sched.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23127"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Dropbox (Energy Innovation)\Documents\EPS_Models by Region\RMI\Virginia\Virginia_Model\InputData\elec\PMCCS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Documents\eps-virginia\InputData\elec\PMCCS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45736304-2D9C-4081-AF78-56563B788BE6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8865" yWindow="465" windowWidth="17340" windowHeight="12825" activeTab="2" xr2:uid="{EDFD5CA4-AA4D-4A6A-B6B7-6C080971D85F}"/>
+    <workbookView xWindow="8865" yWindow="465" windowWidth="17340" windowHeight="12825"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="Required offshore wind" sheetId="3" r:id="rId2"/>
     <sheet name="PMCCS" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -32,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="41">
   <si>
     <t>PMCCS Policy Mandated Capacity Construction Schedule</t>
   </si>
@@ -152,17 +151,20 @@
   </si>
   <si>
     <t>Required offshore wind (MW) Construction</t>
+  </si>
+  <si>
+    <t>Model Chooses to Build Offshore Wind Capacity in the start year, so we must adjust for that here (MW built 2019)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="169" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -205,6 +207,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -239,7 +249,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -257,11 +267,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -270,6 +277,14 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -364,23 +379,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -416,23 +414,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -608,24 +589,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="2" max="2" width="14.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -635,67 +616,67 @@
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B5" s="7">
         <v>43922</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B6" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B8" s="6" t="s">
         <v>32</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B9" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B10" s="7">
         <v>43952</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B11" s="7" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B12" s="7"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>5</v>
       </c>
@@ -707,27 +688,27 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8F4724C-7E44-4AA7-94EC-790A012325F5}">
-  <dimension ref="A1:K47"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="30.5703125" customWidth="1"/>
-    <col min="2" max="2" width="25.42578125" customWidth="1"/>
+    <col min="1" max="1" width="30.59765625" customWidth="1"/>
+    <col min="2" max="2" width="25.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:11" ht="53.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
@@ -735,14 +716,14 @@
       <c r="J1" s="4"/>
       <c r="K1" s="4"/>
     </row>
-    <row r="2" spans="1:11" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
+    <row r="2" spans="1:11" ht="79.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
@@ -750,11 +731,11 @@
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="9"/>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A3" s="8"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
@@ -763,463 +744,514 @@
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+    <row r="4" spans="1:11" ht="35.65" x14ac:dyDescent="0.45">
+      <c r="A4" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A5" s="16">
+        <v>568</v>
+      </c>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A6" s="8"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A9" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A10" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B7">
+      <c r="B10">
+        <f>2600-A5</f>
+        <v>2032</v>
+      </c>
+      <c r="C10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A11" s="3">
+        <v>2026</v>
+      </c>
+      <c r="B11">
+        <f>B12-B10-A5</f>
         <v>2600</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C11" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="10" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
+      <c r="D11" s="9"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A12" s="2">
+        <v>2035</v>
+      </c>
+      <c r="B12">
+        <v>5200</v>
+      </c>
+      <c r="C12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A13" s="2"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A14" s="2"/>
+    </row>
+    <row r="15" spans="1:11" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B15" s="11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="B16" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F16" s="2"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A17">
+        <v>2017</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A18">
+        <v>2018</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A19">
+        <v>2019</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A20">
+        <v>2020</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A21">
+        <v>2021</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A22">
+        <v>2022</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="C22" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A23">
+        <v>2023</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="C23" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A24">
+        <v>2024</v>
+      </c>
+      <c r="B24" s="10">
+        <f>$B$10/3</f>
+        <v>677.33333333333337</v>
+      </c>
+      <c r="C24" s="13">
+        <f>B24</f>
+        <v>677.33333333333337</v>
+      </c>
+      <c r="E24" s="17"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A25">
+        <v>2025</v>
+      </c>
+      <c r="B25" s="10">
+        <f t="shared" ref="B25:B26" si="0">$B$10/3</f>
+        <v>677.33333333333337</v>
+      </c>
+      <c r="C25" s="13">
+        <f>C24+B25</f>
+        <v>1354.6666666666667</v>
+      </c>
+      <c r="E25" s="17"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A26">
         <v>2026</v>
       </c>
-      <c r="B8">
-        <v>2600</v>
-      </c>
-      <c r="C8" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="10"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
+      <c r="B26" s="10">
+        <f t="shared" si="0"/>
+        <v>677.33333333333337</v>
+      </c>
+      <c r="C26" s="13">
+        <f t="shared" ref="C26:C35" si="1">C25+B26</f>
+        <v>2032</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A27">
+        <v>2027</v>
+      </c>
+      <c r="B27" s="10">
+        <f>$B$11/9</f>
+        <v>288.88888888888891</v>
+      </c>
+      <c r="C27" s="13">
+        <f t="shared" si="1"/>
+        <v>2320.8888888888887</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A28">
+        <v>2028</v>
+      </c>
+      <c r="B28" s="10">
+        <f t="shared" ref="B28:B35" si="2">$B$11/9</f>
+        <v>288.88888888888891</v>
+      </c>
+      <c r="C28" s="13">
+        <f t="shared" si="1"/>
+        <v>2609.7777777777774</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A29">
+        <v>2029</v>
+      </c>
+      <c r="B29" s="10">
+        <f t="shared" si="2"/>
+        <v>288.88888888888891</v>
+      </c>
+      <c r="C29" s="13">
+        <f t="shared" si="1"/>
+        <v>2898.6666666666661</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A30">
+        <v>2030</v>
+      </c>
+      <c r="B30" s="10">
+        <f t="shared" si="2"/>
+        <v>288.88888888888891</v>
+      </c>
+      <c r="C30" s="13">
+        <f t="shared" si="1"/>
+        <v>3187.5555555555547</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A31">
+        <v>2031</v>
+      </c>
+      <c r="B31" s="10">
+        <f t="shared" si="2"/>
+        <v>288.88888888888891</v>
+      </c>
+      <c r="C31" s="13">
+        <f t="shared" si="1"/>
+        <v>3476.4444444444434</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A32">
+        <v>2032</v>
+      </c>
+      <c r="B32" s="10">
+        <f t="shared" si="2"/>
+        <v>288.88888888888891</v>
+      </c>
+      <c r="C32" s="13">
+        <f t="shared" si="1"/>
+        <v>3765.3333333333321</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A33">
+        <v>2033</v>
+      </c>
+      <c r="B33" s="10">
+        <f t="shared" si="2"/>
+        <v>288.88888888888891</v>
+      </c>
+      <c r="C33" s="13">
+        <f t="shared" si="1"/>
+        <v>4054.2222222222208</v>
+      </c>
+      <c r="E33" s="18"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A34">
+        <v>2034</v>
+      </c>
+      <c r="B34" s="10">
+        <f t="shared" si="2"/>
+        <v>288.88888888888891</v>
+      </c>
+      <c r="C34" s="13">
+        <f t="shared" si="1"/>
+        <v>4343.1111111111095</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A35">
         <v>2035</v>
       </c>
-      <c r="B9">
-        <v>5200</v>
-      </c>
-      <c r="C9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-    </row>
-    <row r="12" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="B12" s="12" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B13" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F13" s="2"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>2017</v>
-      </c>
-      <c r="B14">
-        <v>0</v>
-      </c>
-      <c r="C14" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>2018</v>
-      </c>
-      <c r="B15">
-        <v>0</v>
-      </c>
-      <c r="C15" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>2019</v>
-      </c>
-      <c r="B16">
-        <v>0</v>
-      </c>
-      <c r="C16" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>2020</v>
-      </c>
-      <c r="B17">
-        <v>0</v>
-      </c>
-      <c r="C17" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>2021</v>
-      </c>
-      <c r="B18">
-        <v>0</v>
-      </c>
-      <c r="C18" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>2022</v>
-      </c>
-      <c r="B19">
-        <v>0</v>
-      </c>
-      <c r="C19" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>2023</v>
-      </c>
-      <c r="B20">
-        <v>0</v>
-      </c>
-      <c r="C20" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>2024</v>
-      </c>
-      <c r="B21" s="11">
-        <f>C21</f>
-        <v>866.66666666666663</v>
-      </c>
-      <c r="C21" s="14">
-        <v>866.66666666666663</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>2025</v>
-      </c>
-      <c r="B22" s="11">
-        <f>C22-C21</f>
-        <v>866.66666666666663</v>
-      </c>
-      <c r="C22" s="14">
-        <v>1733.3333333333333</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>2026</v>
-      </c>
-      <c r="B23" s="11">
-        <f t="shared" ref="B23:B32" si="0">C23-C22</f>
-        <v>866.66666666666674</v>
-      </c>
-      <c r="C23" s="14">
-        <v>2600</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>2027</v>
-      </c>
-      <c r="B24" s="11">
-        <f t="shared" si="0"/>
-        <v>288.88888888887595</v>
-      </c>
-      <c r="C24" s="14">
-        <f>_xlfn.FORECAST.LINEAR(A24,$B$8:$B$9,$A$8:$A$9)</f>
-        <v>2888.888888888876</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>2028</v>
-      </c>
-      <c r="B25" s="11">
-        <f t="shared" si="0"/>
-        <v>288.88888888887595</v>
-      </c>
-      <c r="C25" s="14">
-        <f t="shared" ref="C25:C32" si="1">_xlfn.FORECAST.LINEAR(A25,$B$8:$B$9,$A$8:$A$9)</f>
-        <v>3177.7777777777519</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>2029</v>
-      </c>
-      <c r="B26" s="11">
-        <f t="shared" si="0"/>
-        <v>288.88888888887595</v>
-      </c>
-      <c r="C26" s="14">
-        <f t="shared" si="1"/>
-        <v>3466.6666666666279</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>2030</v>
-      </c>
-      <c r="B27" s="11">
-        <f t="shared" si="0"/>
-        <v>288.88888888887595</v>
-      </c>
-      <c r="C27" s="14">
-        <f t="shared" si="1"/>
-        <v>3755.5555555555038</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>2031</v>
-      </c>
-      <c r="B28" s="11">
-        <f t="shared" si="0"/>
-        <v>288.88888888887595</v>
-      </c>
-      <c r="C28" s="14">
-        <f t="shared" si="1"/>
-        <v>4044.4444444443798</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>2032</v>
-      </c>
-      <c r="B29" s="11">
-        <f t="shared" si="0"/>
-        <v>288.88888888887595</v>
-      </c>
-      <c r="C29" s="14">
-        <f t="shared" si="1"/>
-        <v>4333.3333333332557</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>2033</v>
-      </c>
-      <c r="B30" s="11">
-        <f t="shared" si="0"/>
-        <v>288.88888888887595</v>
-      </c>
-      <c r="C30" s="14">
-        <f t="shared" si="1"/>
-        <v>4622.2222222221317</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>2034</v>
-      </c>
-      <c r="B31" s="11">
-        <f t="shared" si="0"/>
-        <v>288.88888888887595</v>
-      </c>
-      <c r="C31" s="14">
-        <f t="shared" si="1"/>
-        <v>4911.1111111110076</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>2035</v>
-      </c>
-      <c r="B32" s="11">
-        <f t="shared" si="0"/>
-        <v>288.88888888899237</v>
-      </c>
-      <c r="C32" s="14">
-        <f t="shared" si="1"/>
-        <v>5200</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33">
+      <c r="B35" s="10">
+        <f t="shared" si="2"/>
+        <v>288.88888888888891</v>
+      </c>
+      <c r="C35" s="13">
+        <f>C34+B35</f>
+        <v>4631.9999999999982</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A36">
         <v>2036</v>
       </c>
-      <c r="B33">
-        <v>0</v>
-      </c>
-      <c r="C33" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34">
+      <c r="B36">
+        <v>0</v>
+      </c>
+      <c r="C36" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A37">
         <v>2037</v>
       </c>
-      <c r="B34">
-        <v>0</v>
-      </c>
-      <c r="C34" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35">
+      <c r="B37">
+        <v>0</v>
+      </c>
+      <c r="C37" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A38">
         <v>2038</v>
       </c>
-      <c r="B35">
-        <v>0</v>
-      </c>
-      <c r="C35" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36">
+      <c r="B38">
+        <v>0</v>
+      </c>
+      <c r="C38" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A39">
         <v>2039</v>
       </c>
-      <c r="B36">
-        <v>0</v>
-      </c>
-      <c r="C36" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37">
+      <c r="B39">
+        <v>0</v>
+      </c>
+      <c r="C39" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A40">
         <v>2040</v>
       </c>
-      <c r="B37">
-        <v>0</v>
-      </c>
-      <c r="C37" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38">
+      <c r="B40">
+        <v>0</v>
+      </c>
+      <c r="C40" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A41">
         <v>2041</v>
       </c>
-      <c r="B38">
-        <v>0</v>
-      </c>
-      <c r="C38" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39">
+      <c r="B41">
+        <v>0</v>
+      </c>
+      <c r="C41" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A42">
         <v>2042</v>
       </c>
-      <c r="B39">
-        <v>0</v>
-      </c>
-      <c r="C39" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40">
+      <c r="B42">
+        <v>0</v>
+      </c>
+      <c r="C42" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A43">
         <v>2043</v>
       </c>
-      <c r="B40">
-        <v>0</v>
-      </c>
-      <c r="C40" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41">
+      <c r="B43">
+        <v>0</v>
+      </c>
+      <c r="C43" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A44">
         <v>2044</v>
       </c>
-      <c r="B41">
-        <v>0</v>
-      </c>
-      <c r="C41" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42">
+      <c r="B44">
+        <v>0</v>
+      </c>
+      <c r="C44" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A45">
         <v>2045</v>
       </c>
-      <c r="B42">
-        <v>0</v>
-      </c>
-      <c r="C42" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43">
+      <c r="B45">
+        <v>0</v>
+      </c>
+      <c r="C45" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A46">
         <v>2046</v>
       </c>
-      <c r="B43">
-        <v>0</v>
-      </c>
-      <c r="C43" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44">
+      <c r="B46">
+        <v>0</v>
+      </c>
+      <c r="C46" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A47">
         <v>2047</v>
       </c>
-      <c r="B44">
-        <v>0</v>
-      </c>
-      <c r="C44" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45">
+      <c r="B47">
+        <v>0</v>
+      </c>
+      <c r="C47" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A48">
         <v>2048</v>
       </c>
-      <c r="B45">
-        <v>0</v>
-      </c>
-      <c r="C45" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46">
+      <c r="B48">
+        <v>0</v>
+      </c>
+      <c r="C48" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A49">
         <v>2049</v>
       </c>
-      <c r="B46">
-        <v>0</v>
-      </c>
-      <c r="C46" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47">
+      <c r="B49">
+        <v>0</v>
+      </c>
+      <c r="C49" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A50">
         <v>2050</v>
       </c>
-      <c r="B47">
-        <v>0</v>
-      </c>
-      <c r="C47" s="13">
+      <c r="B50">
+        <v>0</v>
+      </c>
+      <c r="C50" s="12">
         <v>0</v>
       </c>
     </row>
@@ -1234,22 +1266,22 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:AI17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="29.5703125" customWidth="1"/>
+    <col min="1" max="1" width="29.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -1356,7 +1388,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -1463,7 +1495,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1570,7 +1602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1677,7 +1709,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -1784,7 +1816,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -1891,7 +1923,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -1998,7 +2030,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -2105,7 +2137,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -2212,7 +2244,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -2319,7 +2351,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -2426,7 +2458,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -2533,7 +2565,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -2640,12 +2672,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>20</v>
       </c>
       <c r="B14">
-        <f t="array" ref="B14:AI14">TRANSPOSE('Required offshore wind'!$B$14:$B$47)</f>
+        <f t="array" ref="B14:AI14">TRANSPOSE('Required offshore wind'!$B$17:$B$50)</f>
         <v>0</v>
       </c>
       <c r="C14">
@@ -2667,40 +2699,40 @@
         <v>0</v>
       </c>
       <c r="I14">
-        <v>866.66666666666663</v>
+        <v>677.33333333333337</v>
       </c>
       <c r="J14">
-        <v>866.66666666666663</v>
+        <v>677.33333333333337</v>
       </c>
       <c r="K14">
-        <v>866.66666666666674</v>
+        <v>677.33333333333337</v>
       </c>
       <c r="L14">
-        <v>288.88888888887595</v>
+        <v>288.88888888888891</v>
       </c>
       <c r="M14">
-        <v>288.88888888887595</v>
+        <v>288.88888888888891</v>
       </c>
       <c r="N14">
-        <v>288.88888888887595</v>
+        <v>288.88888888888891</v>
       </c>
       <c r="O14">
-        <v>288.88888888887595</v>
+        <v>288.88888888888891</v>
       </c>
       <c r="P14">
-        <v>288.88888888887595</v>
+        <v>288.88888888888891</v>
       </c>
       <c r="Q14">
-        <v>288.88888888887595</v>
+        <v>288.88888888888891</v>
       </c>
       <c r="R14">
-        <v>288.88888888887595</v>
+        <v>288.88888888888891</v>
       </c>
       <c r="S14">
-        <v>288.88888888887595</v>
+        <v>288.88888888888891</v>
       </c>
       <c r="T14">
-        <v>288.88888888899237</v>
+        <v>288.88888888888891</v>
       </c>
       <c r="U14">
         <v>0</v>
@@ -2748,7 +2780,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -2855,7 +2887,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -2962,7 +2994,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>23</v>
       </c>

</xml_diff>

<commit_message>
Adjust PMCCS based on recent power sector edits
</commit_message>
<xml_diff>
--- a/InputData/elec/PMCCS/Pol Mandated Cap Const Sched.xlsx
+++ b/InputData/elec/PMCCS/Pol Mandated Cap Const Sched.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="40">
   <si>
     <t>PMCCS Policy Mandated Capacity Construction Schedule</t>
   </si>
@@ -151,9 +151,6 @@
   </si>
   <si>
     <t>Required offshore wind (MW) Construction</t>
-  </si>
-  <si>
-    <t>Model Chooses to Build Offshore Wind Capacity in the start year, so we must adjust for that here (MW built 2019)</t>
   </si>
 </sst>
 </file>
@@ -164,7 +161,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -207,14 +204,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -249,7 +238,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -274,17 +263,14 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -689,10 +675,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K50"/>
+  <dimension ref="A1:K46"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -702,13 +688,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="53.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
@@ -717,13 +703,13 @@
       <c r="K1" s="4"/>
     </row>
     <row r="2" spans="1:11" ht="79.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
@@ -744,119 +730,120 @@
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
     </row>
-    <row r="4" spans="1:11" ht="35.65" x14ac:dyDescent="0.45">
-      <c r="A4" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-    </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A5" s="16">
-        <v>568</v>
-      </c>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
+      <c r="A5" s="1" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A6" s="8"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
+      <c r="A6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6">
+        <f>2600</f>
+        <v>2600</v>
+      </c>
+      <c r="C6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A7" s="3">
+        <v>2026</v>
+      </c>
+      <c r="B7">
+        <f>B8-B6</f>
+        <v>2600</v>
+      </c>
+      <c r="C7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="9"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A8" s="2">
+        <v>2035</v>
+      </c>
+      <c r="B8">
+        <v>5200</v>
+      </c>
+      <c r="C8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A9" s="1" t="s">
-        <v>35</v>
-      </c>
+      <c r="A9" s="2"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A10" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B10">
-        <f>2600-A5</f>
-        <v>2032</v>
-      </c>
-      <c r="C10" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A11" s="3">
-        <v>2026</v>
-      </c>
-      <c r="B11">
-        <f>B12-B10-A5</f>
-        <v>2600</v>
-      </c>
-      <c r="C11" t="s">
-        <v>24</v>
-      </c>
-      <c r="D11" s="9"/>
+      <c r="A10" s="2"/>
+    </row>
+    <row r="11" spans="1:11" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B11" s="11" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A12" s="2">
-        <v>2035</v>
-      </c>
-      <c r="B12">
-        <v>5200</v>
-      </c>
-      <c r="C12" t="s">
-        <v>24</v>
-      </c>
-      <c r="D12" t="s">
-        <v>25</v>
-      </c>
+      <c r="B12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F12" s="2"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A13" s="2"/>
+      <c r="A13">
+        <v>2017</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13" s="12">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A14" s="2"/>
-    </row>
-    <row r="15" spans="1:11" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B15" s="11" t="s">
-        <v>39</v>
+      <c r="A14">
+        <v>2018</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A15">
+        <v>2019</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15" s="12">
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="B16" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F16" s="2"/>
+      <c r="A16">
+        <v>2020</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16" s="12">
+        <v>0</v>
+      </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A17">
-        <v>2017</v>
+        <v>2021</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -867,7 +854,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A18">
-        <v>2018</v>
+        <v>2022</v>
       </c>
       <c r="B18">
         <v>0</v>
@@ -878,7 +865,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A19">
-        <v>2019</v>
+        <v>2023</v>
       </c>
       <c r="B19">
         <v>0</v>
@@ -889,118 +876,126 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A20">
-        <v>2020</v>
-      </c>
-      <c r="B20">
-        <v>0</v>
-      </c>
-      <c r="C20" s="12">
-        <v>0</v>
-      </c>
+        <v>2024</v>
+      </c>
+      <c r="B20" s="10">
+        <f>$B$6/3</f>
+        <v>866.66666666666663</v>
+      </c>
+      <c r="C20" s="13">
+        <f>B20</f>
+        <v>866.66666666666663</v>
+      </c>
+      <c r="E20" s="14"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A21">
-        <v>2021</v>
-      </c>
-      <c r="B21">
-        <v>0</v>
-      </c>
-      <c r="C21" s="12">
-        <v>0</v>
-      </c>
+        <v>2025</v>
+      </c>
+      <c r="B21" s="10">
+        <f t="shared" ref="B21:B22" si="0">$B$6/3</f>
+        <v>866.66666666666663</v>
+      </c>
+      <c r="C21" s="13">
+        <f>C20+B21</f>
+        <v>1733.3333333333333</v>
+      </c>
+      <c r="E21" s="14"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A22">
-        <v>2022</v>
-      </c>
-      <c r="B22">
-        <v>0</v>
-      </c>
-      <c r="C22" s="12">
-        <v>0</v>
+        <v>2026</v>
+      </c>
+      <c r="B22" s="10">
+        <f t="shared" si="0"/>
+        <v>866.66666666666663</v>
+      </c>
+      <c r="C22" s="13">
+        <f t="shared" ref="C22:C30" si="1">C21+B22</f>
+        <v>2600</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A23">
-        <v>2023</v>
-      </c>
-      <c r="B23">
-        <v>0</v>
-      </c>
-      <c r="C23" s="12">
-        <v>0</v>
+        <v>2027</v>
+      </c>
+      <c r="B23" s="10">
+        <f>$B$7/9</f>
+        <v>288.88888888888891</v>
+      </c>
+      <c r="C23" s="13">
+        <f t="shared" si="1"/>
+        <v>2888.8888888888887</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A24">
-        <v>2024</v>
+        <v>2028</v>
       </c>
       <c r="B24" s="10">
-        <f>$B$10/3</f>
-        <v>677.33333333333337</v>
+        <f t="shared" ref="B24:B31" si="2">$B$7/9</f>
+        <v>288.88888888888891</v>
       </c>
       <c r="C24" s="13">
-        <f>B24</f>
-        <v>677.33333333333337</v>
-      </c>
-      <c r="E24" s="17"/>
+        <f t="shared" si="1"/>
+        <v>3177.7777777777774</v>
+      </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A25">
-        <v>2025</v>
+        <v>2029</v>
       </c>
       <c r="B25" s="10">
-        <f t="shared" ref="B25:B26" si="0">$B$10/3</f>
-        <v>677.33333333333337</v>
+        <f t="shared" si="2"/>
+        <v>288.88888888888891</v>
       </c>
       <c r="C25" s="13">
-        <f>C24+B25</f>
-        <v>1354.6666666666667</v>
-      </c>
-      <c r="E25" s="17"/>
+        <f t="shared" si="1"/>
+        <v>3466.6666666666661</v>
+      </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A26">
-        <v>2026</v>
+        <v>2030</v>
       </c>
       <c r="B26" s="10">
-        <f t="shared" si="0"/>
-        <v>677.33333333333337</v>
+        <f t="shared" si="2"/>
+        <v>288.88888888888891</v>
       </c>
       <c r="C26" s="13">
-        <f t="shared" ref="C26:C35" si="1">C25+B26</f>
-        <v>2032</v>
+        <f t="shared" si="1"/>
+        <v>3755.5555555555547</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A27">
-        <v>2027</v>
+        <v>2031</v>
       </c>
       <c r="B27" s="10">
-        <f>$B$11/9</f>
+        <f t="shared" si="2"/>
         <v>288.88888888888891</v>
       </c>
       <c r="C27" s="13">
         <f t="shared" si="1"/>
-        <v>2320.8888888888887</v>
+        <v>4044.4444444444434</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A28">
-        <v>2028</v>
+        <v>2032</v>
       </c>
       <c r="B28" s="10">
-        <f t="shared" ref="B28:B35" si="2">$B$11/9</f>
+        <f t="shared" si="2"/>
         <v>288.88888888888891</v>
       </c>
       <c r="C28" s="13">
         <f t="shared" si="1"/>
-        <v>2609.7777777777774</v>
+        <v>4333.3333333333321</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A29">
-        <v>2029</v>
+        <v>2033</v>
       </c>
       <c r="B29" s="10">
         <f t="shared" si="2"/>
@@ -1008,12 +1003,13 @@
       </c>
       <c r="C29" s="13">
         <f t="shared" si="1"/>
-        <v>2898.6666666666661</v>
-      </c>
+        <v>4622.2222222222208</v>
+      </c>
+      <c r="E29" s="15"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A30">
-        <v>2030</v>
+        <v>2034</v>
       </c>
       <c r="B30" s="10">
         <f t="shared" si="2"/>
@@ -1021,78 +1017,69 @@
       </c>
       <c r="C30" s="13">
         <f t="shared" si="1"/>
-        <v>3187.5555555555547</v>
+        <v>4911.1111111111095</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A31">
-        <v>2031</v>
+        <v>2035</v>
       </c>
       <c r="B31" s="10">
         <f t="shared" si="2"/>
         <v>288.88888888888891</v>
       </c>
       <c r="C31" s="13">
-        <f t="shared" si="1"/>
-        <v>3476.4444444444434</v>
+        <f>C30+B31</f>
+        <v>5199.9999999999982</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A32">
-        <v>2032</v>
-      </c>
-      <c r="B32" s="10">
-        <f t="shared" si="2"/>
-        <v>288.88888888888891</v>
-      </c>
-      <c r="C32" s="13">
-        <f t="shared" si="1"/>
-        <v>3765.3333333333321</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.45">
+        <v>2036</v>
+      </c>
+      <c r="B32">
+        <v>0</v>
+      </c>
+      <c r="C32" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A33">
-        <v>2033</v>
-      </c>
-      <c r="B33" s="10">
-        <f t="shared" si="2"/>
-        <v>288.88888888888891</v>
-      </c>
-      <c r="C33" s="13">
-        <f t="shared" si="1"/>
-        <v>4054.2222222222208</v>
-      </c>
-      <c r="E33" s="18"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.45">
+        <v>2037</v>
+      </c>
+      <c r="B33">
+        <v>0</v>
+      </c>
+      <c r="C33" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A34">
-        <v>2034</v>
-      </c>
-      <c r="B34" s="10">
-        <f t="shared" si="2"/>
-        <v>288.88888888888891</v>
-      </c>
-      <c r="C34" s="13">
-        <f t="shared" si="1"/>
-        <v>4343.1111111111095</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.45">
+        <v>2038</v>
+      </c>
+      <c r="B34">
+        <v>0</v>
+      </c>
+      <c r="C34" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A35">
-        <v>2035</v>
-      </c>
-      <c r="B35" s="10">
-        <f t="shared" si="2"/>
-        <v>288.88888888888891</v>
-      </c>
-      <c r="C35" s="13">
-        <f>C34+B35</f>
-        <v>4631.9999999999982</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.45">
+        <v>2039</v>
+      </c>
+      <c r="B35">
+        <v>0</v>
+      </c>
+      <c r="C35" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A36">
-        <v>2036</v>
+        <v>2040</v>
       </c>
       <c r="B36">
         <v>0</v>
@@ -1101,9 +1088,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A37">
-        <v>2037</v>
+        <v>2041</v>
       </c>
       <c r="B37">
         <v>0</v>
@@ -1112,9 +1099,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A38">
-        <v>2038</v>
+        <v>2042</v>
       </c>
       <c r="B38">
         <v>0</v>
@@ -1123,9 +1110,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A39">
-        <v>2039</v>
+        <v>2043</v>
       </c>
       <c r="B39">
         <v>0</v>
@@ -1134,9 +1121,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A40">
-        <v>2040</v>
+        <v>2044</v>
       </c>
       <c r="B40">
         <v>0</v>
@@ -1145,9 +1132,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A41">
-        <v>2041</v>
+        <v>2045</v>
       </c>
       <c r="B41">
         <v>0</v>
@@ -1156,9 +1143,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A42">
-        <v>2042</v>
+        <v>2046</v>
       </c>
       <c r="B42">
         <v>0</v>
@@ -1167,9 +1154,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A43">
-        <v>2043</v>
+        <v>2047</v>
       </c>
       <c r="B43">
         <v>0</v>
@@ -1178,9 +1165,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A44">
-        <v>2044</v>
+        <v>2048</v>
       </c>
       <c r="B44">
         <v>0</v>
@@ -1189,9 +1176,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A45">
-        <v>2045</v>
+        <v>2049</v>
       </c>
       <c r="B45">
         <v>0</v>
@@ -1200,58 +1187,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A46">
-        <v>2046</v>
+        <v>2050</v>
       </c>
       <c r="B46">
         <v>0</v>
       </c>
       <c r="C46" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A47">
-        <v>2047</v>
-      </c>
-      <c r="B47">
-        <v>0</v>
-      </c>
-      <c r="C47" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A48">
-        <v>2048</v>
-      </c>
-      <c r="B48">
-        <v>0</v>
-      </c>
-      <c r="C48" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A49">
-        <v>2049</v>
-      </c>
-      <c r="B49">
-        <v>0</v>
-      </c>
-      <c r="C49" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A50">
-        <v>2050</v>
-      </c>
-      <c r="B50">
-        <v>0</v>
-      </c>
-      <c r="C50" s="12">
         <v>0</v>
       </c>
     </row>
@@ -2677,7 +2620,7 @@
         <v>20</v>
       </c>
       <c r="B14">
-        <f t="array" ref="B14:AI14">TRANSPOSE('Required offshore wind'!$B$17:$B$50)</f>
+        <f t="array" ref="B14:AI14">TRANSPOSE('Required offshore wind'!$B$13:$B$46)</f>
         <v>0</v>
       </c>
       <c r="C14">
@@ -2699,13 +2642,13 @@
         <v>0</v>
       </c>
       <c r="I14">
-        <v>677.33333333333337</v>
+        <v>866.66666666666663</v>
       </c>
       <c r="J14">
-        <v>677.33333333333337</v>
+        <v>866.66666666666663</v>
       </c>
       <c r="K14">
-        <v>677.33333333333337</v>
+        <v>866.66666666666663</v>
       </c>
       <c r="L14">
         <v>288.88888888888891</v>

</xml_diff>